<commit_message>
name and date in data download
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\DSA\rtp-dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\centers-monitoring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0350D65A-C046-45CB-8A0F-A215A04ABAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3397A3-F097-4421-9A4E-8A3D0576FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74B535C6-8259-44B5-AC9A-6ED9B66D2469}"/>
+    <workbookView xWindow="-30828" yWindow="612" windowWidth="30936" windowHeight="16896" xr2:uid="{74B535C6-8259-44B5-AC9A-6ED9B66D2469}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Notes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,19 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Here is my metadata.</t>
+    <t>Center Name:</t>
   </si>
   <si>
-    <t>Test 1, 2, 3.</t>
+    <t>Date of Download:</t>
+  </si>
+  <si>
+    <t>Census Data Notes:</t>
+  </si>
+  <si>
+    <t>The following data is pulled directly from the US Census Bureau's American Community Survey (ACS):
+     1. Population by Age Group (Table B01001)
+     2. Population by Race and Hispanic Origin (Table B03002)
+     3. Household Income (Table B19001)
+     4. Educational Attainment (Table B15002)
+     5. Housing tenure (Table B25003)
+     6. Housing Unit Type (Table B25004)
+     7. Housing Cost Burden - Renters (Table B25070)
+     8. Housing Cost Burden - Owners (Table B25071)
+     9. Mode to Work for Centers Residents (Table B08301)
+Data for centers is pulled using the Census Bureau's API and is processed by block group. Due to the size of block groups, the only ACS data available is from the 5-year data. For this reason, only non-overlapping five year data sources are shown on the Center's tables. Block groups are then "split" for each center using shares of either population, housing units or households. These shares were generated from a parcelization process that PSRC utilizes using its base-year model parcel inputs and the Office of Financial Management's Small area Estimate Program (SAEP) block data.
+The processing scripts used to pull, clean and organize the Census data is available at: https://github.com/psrc/centers-monitoring/blob/main/pre-process/acs_data_centers.R. Please note that the block group splitting process requires data from the PSRC Central database and as such this script will not run outside the PSRC firewall. If you desire to use a process like this please contact us at info@psrc.org and we will be happy to help you get the data you need to run the process yourself.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,13 +73,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Poppins"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2F1CF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,14 +111,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE2F1CF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -393,25 +443,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECB1712-8E53-4B24-AD2B-29DB072E80EE}">
-  <dimension ref="A1:A3"/>
+  <sheetPr>
+    <tabColor rgb="FFE2F1CF"/>
+  </sheetPr>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21.5" x14ac:dyDescent="0.9"/>
+  <cols>
+    <col min="1" max="1" width="22.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6328125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="10.6328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.9">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final metadata and ui download spacing
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\centers-monitoring\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3397A3-F097-4421-9A4E-8A3D0576FE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E65EA87-A5EF-4E28-BE4A-4C8238B7EF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="612" windowWidth="30936" windowHeight="16896" xr2:uid="{74B535C6-8259-44B5-AC9A-6ED9B66D2469}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Notes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Data Notes'!$1:$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Center Name:</t>
   </si>
@@ -44,7 +47,13 @@
     <t>Date of Download:</t>
   </si>
   <si>
-    <t>Census Data Notes:</t>
+    <t>Travel Model Data</t>
+  </si>
+  <si>
+    <t>Census Data:</t>
+  </si>
+  <si>
+    <t>Employment Data by Sector</t>
   </si>
   <si>
     <t>The following data is pulled directly from the US Census Bureau's American Community Survey (ACS):
@@ -57,8 +66,25 @@
      7. Housing Cost Burden - Renters (Table B25070)
      8. Housing Cost Burden - Owners (Table B25071)
      9. Mode to Work for Centers Residents (Table B08301)
-Data for centers is pulled using the Census Bureau's API and is processed by block group. Due to the size of block groups, the only ACS data available is from the 5-year data. For this reason, only non-overlapping five year data sources are shown on the Center's tables. Block groups are then "split" for each center using shares of either population, housing units or households. These shares were generated from a parcelization process that PSRC utilizes using its base-year model parcel inputs and the Office of Financial Management's Small area Estimate Program (SAEP) block data.
-The processing scripts used to pull, clean and organize the Census data is available at: https://github.com/psrc/centers-monitoring/blob/main/pre-process/acs_data_centers.R. Please note that the block group splitting process requires data from the PSRC Central database and as such this script will not run outside the PSRC firewall. If you desire to use a process like this please contact us at info@psrc.org and we will be happy to help you get the data you need to run the process yourself.</t>
+Data for centers is pulled using the Census Bureau's API and is processed by block group. Due to the size of block groups, the only ACS data available is from the 5-year data. For this reason, only non-overlapping five year data sources are shown on the Center's tables. Block groups are then "split" for each center using shares of either population, housing units or households. These shares were generated from a parcelization process that PSRC utilizes using its base-year model parcel inputs and the Office of Financial Management's Small area Estimate Program (SAEP) block data. The processing scripts used to pull, clean and organize the Census data is available at: https://github.com/psrc/centers-monitoring/blob/main/pre-process/acs_data_centers.R. Please note that the block group splitting process requires data from the PSRC Central database and as such this script will not run outside the PSRC firewall. If you desire to use a process like this please contact us at info@psrc.org and we will be happy to help you get the data you need to run the process yourself.</t>
+  </si>
+  <si>
+    <t>Population, Housing Units and Households:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The following data is pulled from PSRC's latest Activity Based Model (SoundCast) Base Year:
+     1. Destination Mode Share
+     2. Intersection Density
+SoundCast is an Activity Based Model that forecasts detailed travel behavior for individuals on an average weekday.  SoundCast outputs include detailed trip statistics for every person in the region. For purposes of Destination Mode Share in Centers, all trips that fall within a parcel within a given center are aggregated so that a total mode share by center can be calculated. Because SoundCast operates at the parcel level, it takes detailed inputs from Open Street Maps (OSM) which are used to calculate the number of intersections in a specific center. </t>
+  </si>
+  <si>
+    <t>The following derived from the Washington State Employment Security Department (ESD):
+     1. Total Employment
+     2. Job by Sector
+Employment summaries derive from the Quarterly Census of Employment and Wages (QCEW), administrative records employers report, by law, to the Washington State Employment Security Department (ESD).  To provide more accurate workplace reporting, PSRC gathers supplemental data from the Boeing Company, the Office of Washington Superintendent of Public Instruction (OSPI), and governmental units throughout the central Puget Sound region. The unit of measurement is jobs, rather than working persons or proportional full-time employment (FTE) equivalents.  Part-time and temporary positions are included.</t>
+  </si>
+  <si>
+    <t>Total population and housing units are generated using the Office of Financial Management's Small area Estimate Program (SAEP) block data. This data is available by Census block from 2010 through 2022. The blocks are parcelized by PSRC using its base-year model parcel inputs. The parcel centroids that are contained within a given center are aggregated for that center.</t>
   </si>
 </sst>
 </file>
@@ -85,7 +111,7 @@
       <name val="Poppins"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +121,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE2F1CF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3C9E3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBD6C9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFE9E7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -111,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -124,6 +168,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,6 +197,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFE9E7"/>
+      <color rgb="FFFBD6C9"/>
+      <color rgb="FFE3C9E3"/>
       <color rgb="FFE2F1CF"/>
     </mruColors>
   </colors>
@@ -446,7 +514,7 @@
   <sheetPr>
     <tabColor rgb="FFE2F1CF"/>
   </sheetPr>
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -474,211 +542,205 @@
     </row>
     <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
     <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
+      <c r="A4" s="10" t="s">
+        <v>6</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.9">
+      <c r="A12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9"/>
+    <row r="28" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A28" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="A29" s="5"/>
+      <c r="A29" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -709,7 +771,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.9">
+    <row r="33" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -717,12 +779,301 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
+    <row r="34" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+    </row>
+    <row r="39" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+    </row>
+    <row r="48" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+    </row>
+    <row r="49" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+    </row>
+    <row r="50" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+    </row>
+    <row r="51" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+    </row>
+    <row r="52" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+    </row>
+    <row r="57" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A57" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+    </row>
+    <row r="60" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+    </row>
+    <row r="66" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.9">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F33"/>
+    <mergeCell ref="A5:F10"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F25"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A57:F57"/>
+    <mergeCell ref="A58:F69"/>
+    <mergeCell ref="A29:F54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;R&amp;"Poppins,Regular"&amp;10Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="26" max="16383" man="1"/>
+    <brk id="55" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>